<commit_message>
replacing prof_availability and apply_prep!
prof availability is not coherent with the rest
apply_prep! is now outdated
full_filtering! won't find any solution in cases where it should --> to be fixed
</commit_message>
<xml_diff>
--- a/OutputProgram.xlsx
+++ b/OutputProgram.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>Names\Dates</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Galant</t>
-  </si>
-  <si>
-    <t>Exam</t>
   </si>
   <si>
     <t>TN423</t>
@@ -632,9 +629,7 @@
         <v>27</v>
       </c>
       <c r="D2"/>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
+      <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -658,21 +653,17 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3"/>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
@@ -695,21 +686,19 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
+      <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
@@ -730,13 +719,13 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -746,15 +735,9 @@
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" t="s">
-        <v>28</v>
-      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
@@ -769,13 +752,13 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -789,9 +772,7 @@
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
-      <c r="P6" t="s">
-        <v>28</v>
-      </c>
+      <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
       <c r="S6"/>
@@ -804,20 +785,18 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
+      <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -839,17 +818,15 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
@@ -874,21 +851,19 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
+      <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -909,13 +884,13 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -927,9 +902,7 @@
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
-      <c r="N10" t="s">
-        <v>28</v>
-      </c>
+      <c r="N10"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
@@ -944,17 +917,15 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
+      <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -979,13 +950,13 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1002,12 +973,8 @@
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12"/>
-      <c r="S12" t="s">
-        <v>28</v>
-      </c>
-      <c r="T12" t="s">
-        <v>28</v>
-      </c>
+      <c r="S12"/>
+      <c r="T12"/>
       <c r="U12"/>
       <c r="V12"/>
       <c r="W12"/>
@@ -1016,13 +983,13 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1041,25 +1008,21 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
-      <c r="U13" t="s">
-        <v>28</v>
-      </c>
-      <c r="V13" t="s">
-        <v>28</v>
-      </c>
+      <c r="U13"/>
+      <c r="V13"/>
       <c r="W13"/>
       <c r="X13"/>
       <c r="Y13"/>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -1076,12 +1039,8 @@
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
-      <c r="S14" t="s">
-        <v>28</v>
-      </c>
-      <c r="T14" t="s">
-        <v>28</v>
-      </c>
+      <c r="S14"/>
+      <c r="T14"/>
       <c r="U14"/>
       <c r="V14"/>
       <c r="W14"/>
@@ -1090,13 +1049,13 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
@@ -1115,25 +1074,21 @@
       <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
-      <c r="U15" t="s">
-        <v>28</v>
-      </c>
-      <c r="V15" t="s">
-        <v>28</v>
-      </c>
+      <c r="U15"/>
+      <c r="V15"/>
       <c r="W15"/>
       <c r="X15"/>
       <c r="Y15"/>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -1154,9 +1109,7 @@
       <c r="T16"/>
       <c r="U16"/>
       <c r="V16"/>
-      <c r="W16" t="s">
-        <v>28</v>
-      </c>
+      <c r="W16"/>
       <c r="X16"/>
       <c r="Y16"/>
     </row>
@@ -1249,9 +1202,7 @@
         <v>25</v>
       </c>
       <c r="B2"/>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
@@ -1275,337 +1226,9 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3"/>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" t="s">
-        <v>28</v>
-      </c>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9"/>
-      <c r="W9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:W3"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
@@ -1628,155 +1251,11 @@
       <c r="V3"/>
       <c r="W3"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:W6"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-    </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
@@ -1801,7 +1280,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1818,12 +1297,8 @@
       <c r="N5"/>
       <c r="O5"/>
       <c r="P5"/>
-      <c r="Q5" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q5"/>
+      <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
       <c r="U5"/>
@@ -1832,7 +1307,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -1851,12 +1326,446 @@
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
-      <c r="S6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T6" t="s">
-        <v>28</v>
-      </c>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:W6"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
       <c r="U6"/>
       <c r="V6"/>
       <c r="W6"/>

</xml_diff>